<commit_message>
feat(DWG): Finished framework for all I/O modules
</commit_message>
<xml_diff>
--- a/PLC_RTU_Panel/Notes/IO Schedule.xlsx
+++ b/PLC_RTU_Panel/Notes/IO Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zbarge\Documents\Acade 2025\AeData\Proj\32384_CharlesCounty_Pomonkey_PS_Improvements\PLC_RTU_Panel\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1E4AFD-89B9-460D-BC69-866BC9C3A2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEDAA33-5463-418D-9AC4-A76214F45C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -745,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(PLC/RTU DWG):Finished initial draft minus DI modules
</commit_message>
<xml_diff>
--- a/PLC_RTU_Panel/Notes/IO Schedule.xlsx
+++ b/PLC_RTU_Panel/Notes/IO Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zbarge\Documents\Acade 2025\AeData\Proj\32384_CharlesCounty_Pomonkey_PS_Improvements\PLC_RTU_Panel\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEDAA33-5463-418D-9AC4-A76214F45C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EFC0D3-A18C-4AF0-ADB3-373C6E5089F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DBC1BDD1-B910-47A3-AD3E-6AB4F78C1675}" name="Table1" displayName="Table1" ref="A1:G42" totalsRowShown="0">
-  <autoFilter ref="A1:G42" xr:uid="{DBC1BDD1-B910-47A3-AD3E-6AB4F78C1675}"/>
+  <autoFilter ref="A1:G42" xr:uid="{DBC1BDD1-B910-47A3-AD3E-6AB4F78C1675}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="DO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G42">
     <sortCondition ref="C1:C42"/>
   </sortState>
@@ -745,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -782,7 +788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -812,7 +818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -842,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -872,7 +878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -896,7 +902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -916,7 +922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -933,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -950,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -967,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -981,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1018,7 +1024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1052,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1069,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1083,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1225,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1293,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1383,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1453,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1467,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>

</xml_diff>